<commit_message>
Updated CHE_grids model - 2025-08-16 18:31
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
+++ b/VerveStacks_CHE_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional_Trans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{605B3658-F059-4C54-8834-2283282601CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDEEC29E-20E6-4EEF-8A80-D238A017F38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,7 +815,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE505101-64F6-97BB-D594-3EB4F87F94A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EAAED3F-D9E9-46FA-C04F-AE5AE8201F0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>